<commit_message>
Uploading the DataVerse web application
</commit_message>
<xml_diff>
--- a/Excel Files/Traffic_Data_Department_Total.xlsx
+++ b/Excel Files/Traffic_Data_Department_Total.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsoedarnadi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsoedarnadi/Documents/GitHub/Datathon-Dataverse/Excel Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1581EA-CAFD-0D44-B0DC-244F5814824D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C03A2D5-7B92-074D-B261-31BDC4582EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23280" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="13">
   <si>
     <t>Year</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Accident_Count</t>
-  </si>
-  <si>
-    <t>Level</t>
   </si>
   <si>
     <t>Department</t>
@@ -416,17 +413,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="H118" sqref="H118"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -440,11 +437,8 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -460,12 +454,8 @@
       <c r="E2" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F2" t="str">
-        <f>IF(C2&lt;632.25,"LOW",IF(C2&lt;1311.75,"MODERATE","HIGH"))</f>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -481,12 +471,8 @@
       <c r="E3" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F66" si="0">IF(C3&lt;632.25,"LOW",IF(C3&lt;1311.75,"MODERATE","HIGH"))</f>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -502,12 +488,8 @@
       <c r="E4" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F4" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -523,12 +505,8 @@
       <c r="E5" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -544,12 +522,8 @@
       <c r="E6" s="2">
         <v>51.2</v>
       </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -565,12 +539,8 @@
       <c r="E7" s="2">
         <v>51</v>
       </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -586,12 +556,8 @@
       <c r="E8" s="2">
         <v>51.4</v>
       </c>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -607,12 +573,8 @@
       <c r="E9" s="2">
         <v>50.783307000000001</v>
       </c>
-      <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -628,12 +590,8 @@
       <c r="E10" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -649,12 +607,8 @@
       <c r="E11" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -670,12 +624,8 @@
       <c r="E12" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -691,12 +641,8 @@
       <c r="E13" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -712,12 +658,8 @@
       <c r="E14" s="2">
         <v>51.2</v>
       </c>
-      <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -733,12 +675,8 @@
       <c r="E15" s="2">
         <v>51</v>
       </c>
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -754,12 +692,8 @@
       <c r="E16" s="2">
         <v>51.4</v>
       </c>
-      <c r="F16" t="str">
-        <f t="shared" si="0"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -775,12 +709,8 @@
       <c r="E17" s="2">
         <v>50.783307000000001</v>
       </c>
-      <c r="F17" t="str">
-        <f t="shared" si="0"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -796,12 +726,8 @@
       <c r="E18" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
@@ -817,12 +743,8 @@
       <c r="E19" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F19" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -838,12 +760,8 @@
       <c r="E20" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F20" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -859,12 +777,8 @@
       <c r="E21" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F21" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -880,12 +794,8 @@
       <c r="E22" s="2">
         <v>51.2</v>
       </c>
-      <c r="F22" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -901,12 +811,8 @@
       <c r="E23" s="2">
         <v>51</v>
       </c>
-      <c r="F23" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -922,12 +828,8 @@
       <c r="E24" s="2">
         <v>51.4</v>
       </c>
-      <c r="F24" t="str">
-        <f t="shared" si="0"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -943,12 +845,8 @@
       <c r="E25" s="2">
         <v>50.783307000000001</v>
       </c>
-      <c r="F25" t="str">
-        <f t="shared" si="0"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
@@ -964,12 +862,8 @@
       <c r="E26" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F26" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
@@ -985,12 +879,8 @@
       <c r="E27" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F27" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1006,12 +896,8 @@
       <c r="E28" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F28" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -1027,12 +913,8 @@
       <c r="E29" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F29" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -1048,12 +930,8 @@
       <c r="E30" s="2">
         <v>51.2</v>
       </c>
-      <c r="F30" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -1069,12 +947,8 @@
       <c r="E31" s="2">
         <v>51</v>
       </c>
-      <c r="F31" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>9</v>
       </c>
@@ -1090,12 +964,8 @@
       <c r="E32" s="2">
         <v>51.4</v>
       </c>
-      <c r="F32" t="str">
-        <f t="shared" si="0"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -1111,12 +981,8 @@
       <c r="E33" s="2">
         <v>50.783307000000001</v>
       </c>
-      <c r="F33" t="str">
-        <f t="shared" si="0"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -1132,12 +998,8 @@
       <c r="E34" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F34" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
@@ -1153,12 +1015,8 @@
       <c r="E35" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F35" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
@@ -1174,12 +1032,8 @@
       <c r="E36" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F36" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
@@ -1195,12 +1049,8 @@
       <c r="E37" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F37" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
@@ -1216,12 +1066,8 @@
       <c r="E38" s="2">
         <v>51.2</v>
       </c>
-      <c r="F38" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>8</v>
       </c>
@@ -1237,12 +1083,8 @@
       <c r="E39" s="2">
         <v>51</v>
       </c>
-      <c r="F39" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
@@ -1258,12 +1100,8 @@
       <c r="E40" s="2">
         <v>51.4</v>
       </c>
-      <c r="F40" t="str">
-        <f t="shared" si="0"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -1279,12 +1117,8 @@
       <c r="E41" s="2">
         <v>50.783307000000001</v>
       </c>
-      <c r="F41" t="str">
-        <f t="shared" si="0"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>3</v>
       </c>
@@ -1300,12 +1134,8 @@
       <c r="E42" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F42" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>4</v>
       </c>
@@ -1321,12 +1151,8 @@
       <c r="E43" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F43" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
@@ -1342,12 +1168,8 @@
       <c r="E44" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F44" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
@@ -1363,12 +1185,8 @@
       <c r="E45" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F45" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -1384,12 +1202,8 @@
       <c r="E46" s="2">
         <v>51.2</v>
       </c>
-      <c r="F46" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>8</v>
       </c>
@@ -1405,12 +1219,8 @@
       <c r="E47" s="2">
         <v>51</v>
       </c>
-      <c r="F47" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>9</v>
       </c>
@@ -1426,12 +1236,8 @@
       <c r="E48" s="2">
         <v>51.4</v>
       </c>
-      <c r="F48" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
@@ -1447,12 +1253,8 @@
       <c r="E49" s="2">
         <v>50.783307000000001</v>
       </c>
-      <c r="F49" t="str">
-        <f t="shared" si="0"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
@@ -1468,12 +1270,8 @@
       <c r="E50" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F50" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
@@ -1489,12 +1287,8 @@
       <c r="E51" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F51" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>5</v>
       </c>
@@ -1510,12 +1304,8 @@
       <c r="E52" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F52" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>6</v>
       </c>
@@ -1531,12 +1321,8 @@
       <c r="E53" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F53" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
@@ -1552,12 +1338,8 @@
       <c r="E54" s="2">
         <v>51.2</v>
       </c>
-      <c r="F54" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>8</v>
       </c>
@@ -1573,12 +1355,8 @@
       <c r="E55" s="2">
         <v>51</v>
       </c>
-      <c r="F55" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>9</v>
       </c>
@@ -1594,12 +1372,8 @@
       <c r="E56" s="2">
         <v>51.4</v>
       </c>
-      <c r="F56" t="str">
-        <f t="shared" si="0"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>10</v>
       </c>
@@ -1615,12 +1389,8 @@
       <c r="E57" s="2">
         <v>50.783307000000001</v>
       </c>
-      <c r="F57" t="str">
-        <f t="shared" si="0"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>3</v>
       </c>
@@ -1636,12 +1406,8 @@
       <c r="E58" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F58" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>4</v>
       </c>
@@ -1657,12 +1423,8 @@
       <c r="E59" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F59" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>5</v>
       </c>
@@ -1678,12 +1440,8 @@
       <c r="E60" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F60" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>6</v>
       </c>
@@ -1699,12 +1457,8 @@
       <c r="E61" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F61" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -1720,12 +1474,8 @@
       <c r="E62" s="2">
         <v>51.2</v>
       </c>
-      <c r="F62" t="str">
-        <f t="shared" si="0"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>8</v>
       </c>
@@ -1741,12 +1491,8 @@
       <c r="E63" s="2">
         <v>51</v>
       </c>
-      <c r="F63" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>9</v>
       </c>
@@ -1762,12 +1508,8 @@
       <c r="E64" s="2">
         <v>51.4</v>
       </c>
-      <c r="F64" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>10</v>
       </c>
@@ -1783,12 +1525,8 @@
       <c r="E65" s="2">
         <v>50.783307000000001</v>
       </c>
-      <c r="F65" t="str">
-        <f t="shared" si="0"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>3</v>
       </c>
@@ -1804,12 +1542,8 @@
       <c r="E66" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F66" t="str">
-        <f t="shared" si="0"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>4</v>
       </c>
@@ -1825,12 +1559,8 @@
       <c r="E67" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F67" t="str">
-        <f t="shared" ref="F67:F129" si="1">IF(C67&lt;632.25,"LOW",IF(C67&lt;1311.75,"MODERATE","HIGH"))</f>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>5</v>
       </c>
@@ -1846,12 +1576,8 @@
       <c r="E68" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F68" t="str">
-        <f t="shared" si="1"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>6</v>
       </c>
@@ -1867,12 +1593,8 @@
       <c r="E69" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F69" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>7</v>
       </c>
@@ -1888,12 +1610,8 @@
       <c r="E70" s="2">
         <v>51.2</v>
       </c>
-      <c r="F70" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>8</v>
       </c>
@@ -1909,12 +1627,8 @@
       <c r="E71" s="2">
         <v>51</v>
       </c>
-      <c r="F71" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>9</v>
       </c>
@@ -1930,12 +1644,8 @@
       <c r="E72" s="2">
         <v>51.4</v>
       </c>
-      <c r="F72" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>10</v>
       </c>
@@ -1951,12 +1661,8 @@
       <c r="E73" s="2">
         <v>50.783307000000001</v>
       </c>
-      <c r="F73" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>3</v>
       </c>
@@ -1972,12 +1678,8 @@
       <c r="E74" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F74" t="str">
-        <f t="shared" si="1"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>4</v>
       </c>
@@ -1993,12 +1695,8 @@
       <c r="E75" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F75" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>5</v>
       </c>
@@ -2014,12 +1712,8 @@
       <c r="E76" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F76" t="str">
-        <f t="shared" si="1"/>
-        <v>HIGH</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>6</v>
       </c>
@@ -2035,12 +1729,8 @@
       <c r="E77" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F77" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>7</v>
       </c>
@@ -2056,12 +1746,8 @@
       <c r="E78" s="2">
         <v>51.2</v>
       </c>
-      <c r="F78" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>8</v>
       </c>
@@ -2077,12 +1763,8 @@
       <c r="E79" s="2">
         <v>51</v>
       </c>
-      <c r="F79" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>9</v>
       </c>
@@ -2098,12 +1780,8 @@
       <c r="E80" s="2">
         <v>51.4</v>
       </c>
-      <c r="F80" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>10</v>
       </c>
@@ -2119,12 +1797,8 @@
       <c r="E81" s="2">
         <v>50.783307000000001</v>
       </c>
-      <c r="F81" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>3</v>
       </c>
@@ -2140,12 +1814,8 @@
       <c r="E82" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F82" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>4</v>
       </c>
@@ -2161,12 +1831,8 @@
       <c r="E83" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F83" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>5</v>
       </c>
@@ -2182,12 +1848,8 @@
       <c r="E84" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F84" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>6</v>
       </c>
@@ -2203,12 +1865,8 @@
       <c r="E85" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F85" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>7</v>
       </c>
@@ -2224,12 +1882,8 @@
       <c r="E86" s="2">
         <v>51.2</v>
       </c>
-      <c r="F86" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>8</v>
       </c>
@@ -2245,12 +1899,8 @@
       <c r="E87" s="2">
         <v>51</v>
       </c>
-      <c r="F87" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>9</v>
       </c>
@@ -2266,12 +1916,8 @@
       <c r="E88" s="2">
         <v>51.4</v>
       </c>
-      <c r="F88" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>10</v>
       </c>
@@ -2287,12 +1933,8 @@
       <c r="E89" s="2">
         <v>50.783307000000001</v>
       </c>
-      <c r="F89" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>3</v>
       </c>
@@ -2308,12 +1950,8 @@
       <c r="E90" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F90" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>4</v>
       </c>
@@ -2329,12 +1967,8 @@
       <c r="E91" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F91" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>5</v>
       </c>
@@ -2350,12 +1984,8 @@
       <c r="E92" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F92" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>6</v>
       </c>
@@ -2371,12 +2001,8 @@
       <c r="E93" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F93" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>7</v>
       </c>
@@ -2392,12 +2018,8 @@
       <c r="E94" s="2">
         <v>51.2</v>
       </c>
-      <c r="F94" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>8</v>
       </c>
@@ -2413,12 +2035,8 @@
       <c r="E95" s="2">
         <v>51</v>
       </c>
-      <c r="F95" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>9</v>
       </c>
@@ -2434,12 +2052,8 @@
       <c r="E96" s="2">
         <v>51.4</v>
       </c>
-      <c r="F96" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>10</v>
       </c>
@@ -2455,12 +2069,8 @@
       <c r="E97" s="2">
         <v>50.783307000000001</v>
       </c>
-      <c r="F97" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>3</v>
       </c>
@@ -2476,12 +2086,8 @@
       <c r="E98" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F98" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>4</v>
       </c>
@@ -2497,12 +2103,8 @@
       <c r="E99" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F99" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>5</v>
       </c>
@@ -2518,12 +2120,8 @@
       <c r="E100" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F100" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>6</v>
       </c>
@@ -2539,12 +2137,8 @@
       <c r="E101" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F101" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>7</v>
       </c>
@@ -2560,12 +2154,8 @@
       <c r="E102" s="2">
         <v>51.2</v>
       </c>
-      <c r="F102" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>8</v>
       </c>
@@ -2581,12 +2171,8 @@
       <c r="E103" s="2">
         <v>51</v>
       </c>
-      <c r="F103" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>9</v>
       </c>
@@ -2602,12 +2188,8 @@
       <c r="E104" s="2">
         <v>51.4</v>
       </c>
-      <c r="F104" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>10</v>
       </c>
@@ -2623,12 +2205,8 @@
       <c r="E105" s="2">
         <v>50.783307000000001</v>
       </c>
-      <c r="F105" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>3</v>
       </c>
@@ -2644,12 +2222,8 @@
       <c r="E106" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F106" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>4</v>
       </c>
@@ -2665,12 +2239,8 @@
       <c r="E107" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F107" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>5</v>
       </c>
@@ -2686,12 +2256,8 @@
       <c r="E108" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F108" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>6</v>
       </c>
@@ -2707,12 +2273,8 @@
       <c r="E109" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F109" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>7</v>
       </c>
@@ -2728,12 +2290,8 @@
       <c r="E110" s="2">
         <v>51.2</v>
       </c>
-      <c r="F110" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>8</v>
       </c>
@@ -2749,12 +2307,8 @@
       <c r="E111" s="2">
         <v>51</v>
       </c>
-      <c r="F111" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>9</v>
       </c>
@@ -2770,12 +2324,8 @@
       <c r="E112" s="2">
         <v>51.4</v>
       </c>
-      <c r="F112" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>10</v>
       </c>
@@ -2791,12 +2341,8 @@
       <c r="E113" s="2">
         <v>50.783307000000001</v>
       </c>
-      <c r="F113" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>3</v>
       </c>
@@ -2812,12 +2358,8 @@
       <c r="E114" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F114" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>4</v>
       </c>
@@ -2833,12 +2375,8 @@
       <c r="E115" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F115" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>5</v>
       </c>
@@ -2854,12 +2392,8 @@
       <c r="E116" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F116" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>6</v>
       </c>
@@ -2875,12 +2409,8 @@
       <c r="E117" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F117" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>7</v>
       </c>
@@ -2896,12 +2426,8 @@
       <c r="E118" s="2">
         <v>51.2</v>
       </c>
-      <c r="F118" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>8</v>
       </c>
@@ -2917,12 +2443,8 @@
       <c r="E119" s="2">
         <v>51</v>
       </c>
-      <c r="F119" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>9</v>
       </c>
@@ -2938,12 +2460,8 @@
       <c r="E120" s="2">
         <v>51.4</v>
       </c>
-      <c r="F120" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>10</v>
       </c>
@@ -2959,12 +2477,8 @@
       <c r="E121" s="2">
         <v>50.783307000000001</v>
       </c>
-      <c r="F121" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>3</v>
       </c>
@@ -2980,12 +2494,8 @@
       <c r="E122" s="2">
         <v>51.478209999999997</v>
       </c>
-      <c r="F122" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>4</v>
       </c>
@@ -3001,12 +2511,8 @@
       <c r="E123" s="2">
         <v>51.424439999999997</v>
       </c>
-      <c r="F123" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>5</v>
       </c>
@@ -3022,12 +2528,8 @@
       <c r="E124" s="2">
         <v>51.476700000000001</v>
       </c>
-      <c r="F124" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>6</v>
       </c>
@@ -3043,12 +2545,8 @@
       <c r="E125" s="2">
         <v>51.531100000000002</v>
       </c>
-      <c r="F125" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>7</v>
       </c>
@@ -3064,12 +2562,8 @@
       <c r="E126" s="2">
         <v>51.2</v>
       </c>
-      <c r="F126" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>8</v>
       </c>
@@ -3085,12 +2579,8 @@
       <c r="E127" s="2">
         <v>51</v>
       </c>
-      <c r="F127" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>9</v>
       </c>
@@ -3106,12 +2596,8 @@
       <c r="E128" s="2">
         <v>51.4</v>
       </c>
-      <c r="F128" t="str">
-        <f t="shared" si="1"/>
-        <v>MODERATE</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>10</v>
       </c>
@@ -3126,10 +2612,6 @@
       </c>
       <c r="E129" s="2">
         <v>50.783307000000001</v>
-      </c>
-      <c r="F129" t="str">
-        <f t="shared" si="1"/>
-        <v>LOW</v>
       </c>
     </row>
   </sheetData>

</xml_diff>